<commit_message>
Finally, the genetic algorithm is implemented
</commit_message>
<xml_diff>
--- a/full/sliding_window_results_window_1.xlsx
+++ b/full/sliding_window_results_window_1.xlsx
@@ -468,13 +468,13 @@
         <v>28.98</v>
       </c>
       <c r="C2" t="n">
-        <v>27.27367674265432</v>
+        <v>28.61942153242016</v>
       </c>
       <c r="D2" t="n">
-        <v>-1.706323257345677</v>
+        <v>-0.3605784675798382</v>
       </c>
       <c r="E2" t="n">
-        <v>2.91153905855876</v>
+        <v>0.1300168312822245</v>
       </c>
     </row>
     <row r="3">
@@ -485,13 +485,13 @@
         <v>29.15</v>
       </c>
       <c r="C3" t="n">
-        <v>29.95101292305473</v>
+        <v>28.28017903452562</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8010129230547278</v>
+        <v>-0.8698209654743749</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6416217029006793</v>
+        <v>0.7565885119787737</v>
       </c>
     </row>
     <row r="4">
@@ -502,13 +502,13 @@
         <v>29.35</v>
       </c>
       <c r="C4" t="n">
-        <v>32.47735727710793</v>
+        <v>28.88646415724472</v>
       </c>
       <c r="D4" t="n">
-        <v>3.127357277107926</v>
+        <v>-0.4635358427552845</v>
       </c>
       <c r="E4" t="n">
-        <v>9.7803635386799</v>
+        <v>0.2148654775188518</v>
       </c>
     </row>
     <row r="5">
@@ -519,13 +519,13 @@
         <v>29.37</v>
       </c>
       <c r="C5" t="n">
-        <v>40.53458207152657</v>
+        <v>28.79124348772752</v>
       </c>
       <c r="D5" t="n">
-        <v>11.16458207152657</v>
+        <v>-0.5787565122724807</v>
       </c>
       <c r="E5" t="n">
-        <v>124.6478928318525</v>
+        <v>0.3349591004978061</v>
       </c>
     </row>
     <row r="6">
@@ -536,13 +536,13 @@
         <v>29.54</v>
       </c>
       <c r="C6" t="n">
-        <v>32.04864912810361</v>
+        <v>28.69696473790746</v>
       </c>
       <c r="D6" t="n">
-        <v>2.508649128103613</v>
+        <v>-0.8430352620925348</v>
       </c>
       <c r="E6" t="n">
-        <v>6.293320447935018</v>
+        <v>0.7107084531314288</v>
       </c>
     </row>
     <row r="7">
@@ -553,13 +553,13 @@
         <v>29.55</v>
       </c>
       <c r="C7" t="n">
-        <v>33.04873516422741</v>
+        <v>29.86126388352603</v>
       </c>
       <c r="D7" t="n">
-        <v>3.498735164227408</v>
+        <v>0.3112638835260277</v>
       </c>
       <c r="E7" t="n">
-        <v>12.24114774940139</v>
+        <v>0.09688520518770456</v>
       </c>
     </row>
     <row r="8">
@@ -570,13 +570,13 @@
         <v>29.75</v>
       </c>
       <c r="C8" t="n">
-        <v>26.933526309154</v>
+        <v>29.59043104121293</v>
       </c>
       <c r="D8" t="n">
-        <v>-2.816473690846003</v>
+        <v>-0.1595689587870659</v>
       </c>
       <c r="E8" t="n">
-        <v>7.932524051227706</v>
+        <v>0.02546225260838833</v>
       </c>
     </row>
     <row r="9">
@@ -587,13 +587,13 @@
         <v>29.84</v>
       </c>
       <c r="C9" t="n">
-        <v>31.6276209587373</v>
+        <v>30.47360527894018</v>
       </c>
       <c r="D9" t="n">
-        <v>1.787620958737303</v>
+        <v>0.6336052789401769</v>
       </c>
       <c r="E9" t="n">
-        <v>3.195588692116876</v>
+        <v>0.4014556495008594</v>
       </c>
     </row>
     <row r="10">
@@ -604,13 +604,13 @@
         <v>29.81</v>
       </c>
       <c r="C10" t="n">
-        <v>36.49610617874655</v>
+        <v>30.35429894197885</v>
       </c>
       <c r="D10" t="n">
-        <v>6.686106178746552</v>
+        <v>0.5442989419788482</v>
       </c>
       <c r="E10" t="n">
-        <v>44.70401583347282</v>
+        <v>0.2962613382392936</v>
       </c>
     </row>
     <row r="11">
@@ -621,13 +621,13 @@
         <v>29.92</v>
       </c>
       <c r="C11" t="n">
-        <v>32.40153223851085</v>
+        <v>30.19960459309228</v>
       </c>
       <c r="D11" t="n">
-        <v>2.481532238510852</v>
+        <v>0.2796045930922801</v>
       </c>
       <c r="E11" t="n">
-        <v>6.158002250768678</v>
+        <v>0.07817872847829956</v>
       </c>
     </row>
     <row r="12">
@@ -638,13 +638,13 @@
         <v>29.98</v>
       </c>
       <c r="C12" t="n">
-        <v>32.59777941067917</v>
+        <v>29.54863326317109</v>
       </c>
       <c r="D12" t="n">
-        <v>2.617779410679166</v>
+        <v>-0.4313667368289096</v>
       </c>
       <c r="E12" t="n">
-        <v>6.852769042975761</v>
+        <v>0.1860772616424217</v>
       </c>
     </row>
     <row r="13">
@@ -655,13 +655,13 @@
         <v>30.04</v>
       </c>
       <c r="C13" t="n">
-        <v>31.56014364349927</v>
+        <v>29.85653219908905</v>
       </c>
       <c r="D13" t="n">
-        <v>1.520143643499267</v>
+        <v>-0.1834678009109503</v>
       </c>
       <c r="E13" t="n">
-        <v>2.310836696871227</v>
+        <v>0.03366043397110009</v>
       </c>
     </row>
     <row r="14">
@@ -672,13 +672,13 @@
         <v>30.21</v>
       </c>
       <c r="C14" t="n">
-        <v>26.57097416083952</v>
+        <v>29.40461724422588</v>
       </c>
       <c r="D14" t="n">
-        <v>-3.639025839160485</v>
+        <v>-0.8053827557741222</v>
       </c>
       <c r="E14" t="n">
-        <v>13.24250905807767</v>
+        <v>0.6486413832983194</v>
       </c>
     </row>
     <row r="15">
@@ -689,13 +689,13 @@
         <v>30.22</v>
       </c>
       <c r="C15" t="n">
-        <v>30.59178170037676</v>
+        <v>29.82918319365324</v>
       </c>
       <c r="D15" t="n">
-        <v>0.3717817003767614</v>
+        <v>-0.3908168063467627</v>
       </c>
       <c r="E15" t="n">
-        <v>0.138221632735036</v>
+        <v>0.1527377761230831</v>
       </c>
     </row>
     <row r="16">
@@ -706,13 +706,13 @@
         <v>30.38</v>
       </c>
       <c r="C16" t="n">
-        <v>26.0835746947615</v>
+        <v>29.64636299647648</v>
       </c>
       <c r="D16" t="n">
-        <v>-4.296425305238504</v>
+        <v>-0.7336370035235191</v>
       </c>
       <c r="E16" t="n">
-        <v>18.45927040349377</v>
+        <v>0.538223252938968</v>
       </c>
     </row>
     <row r="17">
@@ -723,13 +723,13 @@
         <v>30.44</v>
       </c>
       <c r="C17" t="n">
-        <v>28.85308941879928</v>
+        <v>30.33773402865503</v>
       </c>
       <c r="D17" t="n">
-        <v>-1.586910581200726</v>
+        <v>-0.1022659713449734</v>
       </c>
       <c r="E17" t="n">
-        <v>2.518285192726827</v>
+        <v>0.01045832889513092</v>
       </c>
     </row>
     <row r="18">
@@ -740,13 +740,13 @@
         <v>30.48</v>
       </c>
       <c r="C18" t="n">
-        <v>30.56848877019742</v>
+        <v>30.36049336566984</v>
       </c>
       <c r="D18" t="n">
-        <v>0.08848877019741508</v>
+        <v>-0.1195066343301612</v>
       </c>
       <c r="E18" t="n">
-        <v>0.007830262451050935</v>
+        <v>0.01428183564892286</v>
       </c>
     </row>
     <row r="19">
@@ -757,13 +757,13 @@
         <v>30.69</v>
       </c>
       <c r="C19" t="n">
-        <v>26.27699389682165</v>
+        <v>30.65505704903011</v>
       </c>
       <c r="D19" t="n">
-        <v>-4.413006103178351</v>
+        <v>-0.03494295096988864</v>
       </c>
       <c r="E19" t="n">
-        <v>19.47462286668937</v>
+        <v>0.001221009822484041</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +774,13 @@
         <v>30.75</v>
       </c>
       <c r="C20" t="n">
-        <v>29.95621783596824</v>
+        <v>30.32258370656307</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.7937821640317573</v>
+        <v>-0.4274162934369308</v>
       </c>
       <c r="E20" t="n">
-        <v>0.6300901239349396</v>
+        <v>0.1826846878953645</v>
       </c>
     </row>
     <row r="21">
@@ -791,13 +791,13 @@
         <v>30.94</v>
       </c>
       <c r="C21" t="n">
-        <v>27.70240447737902</v>
+        <v>30.73581033191036</v>
       </c>
       <c r="D21" t="n">
-        <v>-3.237595522620985</v>
+        <v>-0.2041896680896436</v>
       </c>
       <c r="E21" t="n">
-        <v>10.48202476809545</v>
+        <v>0.0416934205545588</v>
       </c>
     </row>
     <row r="22">
@@ -808,13 +808,13 @@
         <v>30.95</v>
       </c>
       <c r="C22" t="n">
-        <v>31.9041883626221</v>
+        <v>31.06682419096773</v>
       </c>
       <c r="D22" t="n">
-        <v>0.9541883626220979</v>
+        <v>0.1168241909677299</v>
       </c>
       <c r="E22" t="n">
-        <v>0.9104754313634402</v>
+        <v>0.01364789159526462</v>
       </c>
     </row>
     <row r="23">
@@ -825,13 +825,13 @@
         <v>31.02</v>
       </c>
       <c r="C23" t="n">
-        <v>29.23776339924621</v>
+        <v>31.71203661379989</v>
       </c>
       <c r="D23" t="n">
-        <v>-1.782236600753787</v>
+        <v>0.692036613799889</v>
       </c>
       <c r="E23" t="n">
-        <v>3.176367301066415</v>
+        <v>0.4789146748396167</v>
       </c>
     </row>
     <row r="24">
@@ -842,13 +842,13 @@
         <v>31.12</v>
       </c>
       <c r="C24" t="n">
-        <v>28.03294748997678</v>
+        <v>32.12226057527928</v>
       </c>
       <c r="D24" t="n">
-        <v>-3.087052510023216</v>
+        <v>1.002260575279283</v>
       </c>
       <c r="E24" t="n">
-        <v>9.529893199640641</v>
+        <v>1.00452626075916</v>
       </c>
     </row>
     <row r="25">
@@ -859,13 +859,13 @@
         <v>31.28</v>
       </c>
       <c r="C25" t="n">
-        <v>27.54646528747271</v>
+        <v>32.26900250503424</v>
       </c>
       <c r="D25" t="n">
-        <v>-3.733534712527291</v>
+        <v>0.989002505034243</v>
       </c>
       <c r="E25" t="n">
-        <v>13.93928144964624</v>
+        <v>0.9781259549640079</v>
       </c>
     </row>
     <row r="26">
@@ -876,13 +876,13 @@
         <v>31.38</v>
       </c>
       <c r="C26" t="n">
-        <v>29.34846520023044</v>
+        <v>32.11758947928325</v>
       </c>
       <c r="D26" t="n">
-        <v>-2.031534799769556</v>
+        <v>0.7375894792832476</v>
       </c>
       <c r="E26" t="n">
-        <v>4.12713364267473</v>
+        <v>0.5440382399493323</v>
       </c>
     </row>
     <row r="27">
@@ -893,13 +893,13 @@
         <v>31.58</v>
       </c>
       <c r="C27" t="n">
-        <v>25.61536729262351</v>
+        <v>32.53827326168924</v>
       </c>
       <c r="D27" t="n">
-        <v>-5.964632707376484</v>
+        <v>0.9582732616892429</v>
       </c>
       <c r="E27" t="n">
-        <v>35.57684333390533</v>
+        <v>0.9182876440685401</v>
       </c>
     </row>
     <row r="28">
@@ -910,13 +910,13 @@
         <v>31.65</v>
       </c>
       <c r="C28" t="n">
-        <v>27.53053414009466</v>
+        <v>32.52980955291806</v>
       </c>
       <c r="D28" t="n">
-        <v>-4.11946585990534</v>
+        <v>0.8798095529180614</v>
       </c>
       <c r="E28" t="n">
-        <v>16.96999897092564</v>
+        <v>0.7740648494058791</v>
       </c>
     </row>
     <row r="29">
@@ -927,13 +927,13 @@
         <v>31.88</v>
       </c>
       <c r="C29" t="n">
-        <v>23.66947265602283</v>
+        <v>33.277970159239</v>
       </c>
       <c r="D29" t="n">
-        <v>-8.210527343977169</v>
+        <v>1.397970159238998</v>
       </c>
       <c r="E29" t="n">
-        <v>67.41275926619679</v>
+        <v>1.954320566122709</v>
       </c>
     </row>
     <row r="30">
@@ -944,13 +944,13 @@
         <v>32.28</v>
       </c>
       <c r="C30" t="n">
-        <v>19.18077357617441</v>
+        <v>32.85379537904976</v>
       </c>
       <c r="D30" t="n">
-        <v>-13.09922642382559</v>
+        <v>0.5737953790497556</v>
       </c>
       <c r="E30" t="n">
-        <v>171.5897329026505</v>
+        <v>0.3292411370188528</v>
       </c>
     </row>
     <row r="31">
@@ -961,13 +961,13 @@
         <v>32.45</v>
       </c>
       <c r="C31" t="n">
-        <v>24.32805805250724</v>
+        <v>32.96916922584683</v>
       </c>
       <c r="D31" t="n">
-        <v>-8.121941947492761</v>
+        <v>0.5191692258468237</v>
       </c>
       <c r="E31" t="n">
-        <v>65.96594099844251</v>
+        <v>0.2695366850663902</v>
       </c>
     </row>
     <row r="32">
@@ -978,13 +978,13 @@
         <v>32.85</v>
       </c>
       <c r="C32" t="n">
-        <v>20.18080362030324</v>
+        <v>33.13367271978353</v>
       </c>
       <c r="D32" t="n">
-        <v>-12.66919637969676</v>
+        <v>0.2836727197835245</v>
       </c>
       <c r="E32" t="n">
-        <v>160.5085369073215</v>
+        <v>0.080470211949382</v>
       </c>
     </row>
     <row r="33">
@@ -995,13 +995,13 @@
         <v>32.9</v>
       </c>
       <c r="C33" t="n">
-        <v>28.61768394061367</v>
+        <v>33.22534331497836</v>
       </c>
       <c r="D33" t="n">
-        <v>-4.282316059386332</v>
+        <v>0.3253433149783618</v>
       </c>
       <c r="E33" t="n">
-        <v>18.33823083247808</v>
+        <v>0.1058482726011095</v>
       </c>
     </row>
     <row r="34">
@@ -1012,13 +1012,13 @@
         <v>33.1</v>
       </c>
       <c r="C34" t="n">
-        <v>19.16108994706998</v>
+        <v>33.21840007594129</v>
       </c>
       <c r="D34" t="n">
-        <v>-13.93891005293002</v>
+        <v>0.1184000759412882</v>
       </c>
       <c r="E34" t="n">
-        <v>194.2932134636737</v>
+        <v>0.01401857798290281</v>
       </c>
     </row>
     <row r="35">
@@ -1029,13 +1029,13 @@
         <v>33.4</v>
       </c>
       <c r="C35" t="n">
-        <v>15.1235905057676</v>
+        <v>34.21330507641433</v>
       </c>
       <c r="D35" t="n">
-        <v>-18.2764094942324</v>
+        <v>0.8133050764143306</v>
       </c>
       <c r="E35" t="n">
-        <v>334.0271440008681</v>
+        <v>0.6614651473213201</v>
       </c>
     </row>
     <row r="36">
@@ -1046,13 +1046,13 @@
         <v>33.7</v>
       </c>
       <c r="C36" t="n">
-        <v>17.40542758132423</v>
+        <v>33.99777500965789</v>
       </c>
       <c r="D36" t="n">
-        <v>-16.29457241867578</v>
+        <v>0.2977750096578902</v>
       </c>
       <c r="E36" t="n">
-        <v>265.5130903074694</v>
+        <v>0.08866995637675658</v>
       </c>
     </row>
     <row r="37">
@@ -1063,13 +1063,13 @@
         <v>34.1</v>
       </c>
       <c r="C37" t="n">
-        <v>17.29317257860101</v>
+        <v>34.04644958257992</v>
       </c>
       <c r="D37" t="n">
-        <v>-16.80682742139899</v>
+        <v>-0.05355041742008382</v>
       </c>
       <c r="E37" t="n">
-        <v>282.469447972689</v>
+        <v>0.002867647205865216</v>
       </c>
     </row>
     <row r="38">
@@ -1080,13 +1080,13 @@
         <v>34.4</v>
       </c>
       <c r="C38" t="n">
-        <v>19.73721875466109</v>
+        <v>34.57601968097843</v>
       </c>
       <c r="D38" t="n">
-        <v>-14.66278124533891</v>
+        <v>0.1760196809784276</v>
       </c>
       <c r="E38" t="n">
-        <v>214.9971538486625</v>
+        <v>0.03098292809174742</v>
       </c>
     </row>
     <row r="39">
@@ -1097,13 +1097,13 @@
         <v>34.9</v>
       </c>
       <c r="C39" t="n">
-        <v>16.22969319967525</v>
+        <v>34.85083618170182</v>
       </c>
       <c r="D39" t="n">
-        <v>-18.67030680032475</v>
+        <v>-0.04916381829818306</v>
       </c>
       <c r="E39" t="n">
-        <v>348.5803560182524</v>
+        <v>0.002417081029656759</v>
       </c>
     </row>
     <row r="40">
@@ -1114,13 +1114,13 @@
         <v>35.3</v>
       </c>
       <c r="C40" t="n">
-        <v>17.13561827025836</v>
+        <v>35.9687543924692</v>
       </c>
       <c r="D40" t="n">
-        <v>-18.16438172974164</v>
+        <v>0.6687543924692037</v>
       </c>
       <c r="E40" t="n">
-        <v>329.9447636237718</v>
+        <v>0.4472324374468536</v>
       </c>
     </row>
     <row r="41">
@@ -1131,13 +1131,13 @@
         <v>35.7</v>
       </c>
       <c r="C41" t="n">
-        <v>19.72627297554938</v>
+        <v>36.10000759518975</v>
       </c>
       <c r="D41" t="n">
-        <v>-15.97372702445062</v>
+        <v>0.4000075951897486</v>
       </c>
       <c r="E41" t="n">
-        <v>255.1599550516641</v>
+        <v>0.1600060762094858</v>
       </c>
     </row>
     <row r="42">
@@ -1148,13 +1148,13 @@
         <v>36.3</v>
       </c>
       <c r="C42" t="n">
-        <v>16.98632978352722</v>
+        <v>35.91907778380174</v>
       </c>
       <c r="D42" t="n">
-        <v>-19.31367021647278</v>
+        <v>-0.3809222161982575</v>
       </c>
       <c r="E42" t="n">
-        <v>373.0178572306676</v>
+        <v>0.145101734793392</v>
       </c>
     </row>
     <row r="43">
@@ -1165,13 +1165,13 @@
         <v>36.8</v>
       </c>
       <c r="C43" t="n">
-        <v>20.52863756746252</v>
+        <v>36.40238053655096</v>
       </c>
       <c r="D43" t="n">
-        <v>-16.27136243253748</v>
+        <v>-0.3976194634490327</v>
       </c>
       <c r="E43" t="n">
-        <v>264.757235410992</v>
+        <v>0.1581012377134966</v>
       </c>
     </row>
     <row r="44">
@@ -1182,13 +1182,13 @@
         <v>37.3</v>
       </c>
       <c r="C44" t="n">
-        <v>23.42693962853331</v>
+        <v>36.34026366487587</v>
       </c>
       <c r="D44" t="n">
-        <v>-13.87306037146669</v>
+        <v>-0.959736335124127</v>
       </c>
       <c r="E44" t="n">
-        <v>192.4618040703595</v>
+        <v>0.9210938329574907</v>
       </c>
     </row>
     <row r="45">
@@ -1199,13 +1199,13 @@
         <v>37.9</v>
       </c>
       <c r="C45" t="n">
-        <v>25.35499569832139</v>
+        <v>37.45542092048556</v>
       </c>
       <c r="D45" t="n">
-        <v>-12.54500430167861</v>
+        <v>-0.4445790795144404</v>
       </c>
       <c r="E45" t="n">
-        <v>157.3771329291349</v>
+        <v>0.1976505579419071</v>
       </c>
     </row>
     <row r="46">
@@ -1216,13 +1216,13 @@
         <v>38.5</v>
       </c>
       <c r="C46" t="n">
-        <v>23.94532096679433</v>
+        <v>38.17963449233827</v>
       </c>
       <c r="D46" t="n">
-        <v>-14.55467903320567</v>
+        <v>-0.3203655076617338</v>
       </c>
       <c r="E46" t="n">
-        <v>211.8386817596366</v>
+        <v>0.1026340584993604</v>
       </c>
     </row>
     <row r="47">
@@ -1233,13 +1233,13 @@
         <v>38.9</v>
       </c>
       <c r="C47" t="n">
-        <v>29.02662866392001</v>
+        <v>38.58431861107851</v>
       </c>
       <c r="D47" t="n">
-        <v>-9.873371336079984</v>
+        <v>-0.3156813889214902</v>
       </c>
       <c r="E47" t="n">
-        <v>97.48346154012584</v>
+        <v>0.09965473931140117</v>
       </c>
     </row>
     <row r="48">
@@ -1250,13 +1250,13 @@
         <v>39.4</v>
       </c>
       <c r="C48" t="n">
-        <v>26.63026403997198</v>
+        <v>38.90683823342697</v>
       </c>
       <c r="D48" t="n">
-        <v>-12.76973596002802</v>
+        <v>-0.4931617665730244</v>
       </c>
       <c r="E48" t="n">
-        <v>163.0661564888327</v>
+        <v>0.2432085280094262</v>
       </c>
     </row>
     <row r="49">
@@ -1267,13 +1267,13 @@
         <v>39.9</v>
       </c>
       <c r="C49" t="n">
-        <v>23.34912402302717</v>
+        <v>39.41233102678765</v>
       </c>
       <c r="D49" t="n">
-        <v>-16.55087597697283</v>
+        <v>-0.4876689732123509</v>
       </c>
       <c r="E49" t="n">
-        <v>273.9314956051362</v>
+        <v>0.2378210274339886</v>
       </c>
     </row>
     <row r="50">
@@ -1284,13 +1284,13 @@
         <v>40.1</v>
       </c>
       <c r="C50" t="n">
-        <v>23.9661379042276</v>
+        <v>39.24870500583931</v>
       </c>
       <c r="D50" t="n">
-        <v>-16.1338620957724</v>
+        <v>-0.8512949941606962</v>
       </c>
       <c r="E50" t="n">
-        <v>260.3015061254014</v>
+        <v>0.7247031670830598</v>
       </c>
     </row>
     <row r="51">
@@ -1301,13 +1301,13 @@
         <v>40.6</v>
       </c>
       <c r="C51" t="n">
-        <v>23.08334523113383</v>
+        <v>39.33456577636483</v>
       </c>
       <c r="D51" t="n">
-        <v>-17.51665476886618</v>
+        <v>-1.265434223635175</v>
       </c>
       <c r="E51" t="n">
-        <v>306.8331942916421</v>
+        <v>1.601323774347159</v>
       </c>
     </row>
     <row r="52">
@@ -1318,11 +1318,11 @@
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="n">
-        <v>-334.1734226611409</v>
+        <v>-0.008685308628653132</v>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>5386.721320180256</v>
+        <v>18.1450358373095</v>
       </c>
     </row>
     <row r="53">
@@ -1335,7 +1335,7 @@
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>107.7344264036051</v>
+        <v>0.36290071674619</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor code to save results in a specified folder
</commit_message>
<xml_diff>
--- a/full/sliding_window_results_window_1.xlsx
+++ b/full/sliding_window_results_window_1.xlsx
@@ -468,13 +468,13 @@
         <v>28.98</v>
       </c>
       <c r="C2" t="n">
-        <v>28.61942153242016</v>
+        <v>27.49241226758658</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.3605784675798382</v>
+        <v>-1.48758773241342</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1300168312822245</v>
+        <v>2.212917261626901</v>
       </c>
     </row>
     <row r="3">
@@ -485,13 +485,13 @@
         <v>29.15</v>
       </c>
       <c r="C3" t="n">
-        <v>28.28017903452562</v>
+        <v>28.1808189083947</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.8698209654743749</v>
+        <v>-0.9691810916053001</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7565885119787737</v>
+        <v>0.9393119883252411</v>
       </c>
     </row>
     <row r="4">
@@ -502,13 +502,13 @@
         <v>29.35</v>
       </c>
       <c r="C4" t="n">
-        <v>28.88646415724472</v>
+        <v>29.85633800906434</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.4635358427552845</v>
+        <v>0.5063380090643363</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2148654775188518</v>
+        <v>0.2563781794232359</v>
       </c>
     </row>
     <row r="5">
@@ -519,13 +519,13 @@
         <v>29.37</v>
       </c>
       <c r="C5" t="n">
-        <v>28.79124348772752</v>
+        <v>29.60282396639035</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.5787565122724807</v>
+        <v>0.2328239663903524</v>
       </c>
       <c r="E5" t="n">
-        <v>0.3349591004978061</v>
+        <v>0.05420699932573595</v>
       </c>
     </row>
     <row r="6">
@@ -536,13 +536,13 @@
         <v>29.54</v>
       </c>
       <c r="C6" t="n">
-        <v>28.69696473790746</v>
+        <v>29.15167570878408</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.8430352620925348</v>
+        <v>-0.3883242912159233</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7107084531314288</v>
+        <v>0.1507957551483492</v>
       </c>
     </row>
     <row r="7">
@@ -553,13 +553,13 @@
         <v>29.55</v>
       </c>
       <c r="C7" t="n">
-        <v>29.86126388352603</v>
+        <v>28.50871812765812</v>
       </c>
       <c r="D7" t="n">
-        <v>0.3112638835260277</v>
+        <v>-1.04128187234188</v>
       </c>
       <c r="E7" t="n">
-        <v>0.09688520518770456</v>
+        <v>1.084267937667812</v>
       </c>
     </row>
     <row r="8">
@@ -570,13 +570,13 @@
         <v>29.75</v>
       </c>
       <c r="C8" t="n">
-        <v>29.59043104121293</v>
+        <v>29.53306944917504</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1595689587870659</v>
+        <v>-0.2169305508249622</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02546225260838833</v>
+        <v>0.04705886388122149</v>
       </c>
     </row>
     <row r="9">
@@ -587,13 +587,13 @@
         <v>29.84</v>
       </c>
       <c r="C9" t="n">
-        <v>30.47360527894018</v>
+        <v>30.23630653117635</v>
       </c>
       <c r="D9" t="n">
-        <v>0.6336052789401769</v>
+        <v>0.3963065311763465</v>
       </c>
       <c r="E9" t="n">
-        <v>0.4014556495008594</v>
+        <v>0.1570588666530285</v>
       </c>
     </row>
     <row r="10">
@@ -604,13 +604,13 @@
         <v>29.81</v>
       </c>
       <c r="C10" t="n">
-        <v>30.35429894197885</v>
+        <v>29.98318372129723</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5442989419788482</v>
+        <v>0.1731837212972316</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2962613382392936</v>
+        <v>0.02999260132235718</v>
       </c>
     </row>
     <row r="11">
@@ -621,13 +621,13 @@
         <v>29.92</v>
       </c>
       <c r="C11" t="n">
-        <v>30.19960459309228</v>
+        <v>31.1543561372367</v>
       </c>
       <c r="D11" t="n">
-        <v>0.2796045930922801</v>
+        <v>1.234356137236695</v>
       </c>
       <c r="E11" t="n">
-        <v>0.07817872847829956</v>
+        <v>1.523635073533894</v>
       </c>
     </row>
     <row r="12">
@@ -638,13 +638,13 @@
         <v>29.98</v>
       </c>
       <c r="C12" t="n">
-        <v>29.54863326317109</v>
+        <v>29.96703474200553</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.4313667368289096</v>
+        <v>-0.01296525799446968</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1860772616424217</v>
+        <v>0.00016809791486316</v>
       </c>
     </row>
     <row r="13">
@@ -655,13 +655,13 @@
         <v>30.04</v>
       </c>
       <c r="C13" t="n">
-        <v>29.85653219908905</v>
+        <v>30.03303552117937</v>
       </c>
       <c r="D13" t="n">
-        <v>-0.1834678009109503</v>
+        <v>-0.006964478820627562</v>
       </c>
       <c r="E13" t="n">
-        <v>0.03366043397110009</v>
+        <v>4.850396524296988e-05</v>
       </c>
     </row>
     <row r="14">
@@ -672,13 +672,13 @@
         <v>30.21</v>
       </c>
       <c r="C14" t="n">
-        <v>29.40461724422588</v>
+        <v>30.09177113028868</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.8053827557741222</v>
+        <v>-0.1182288697113236</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6486413832983194</v>
+        <v>0.01397806563321714</v>
       </c>
     </row>
     <row r="15">
@@ -689,13 +689,13 @@
         <v>30.22</v>
       </c>
       <c r="C15" t="n">
-        <v>29.82918319365324</v>
+        <v>29.59311683979067</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.3908168063467627</v>
+        <v>-0.6268831602093314</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1527377761230831</v>
+        <v>0.3929824965540383</v>
       </c>
     </row>
     <row r="16">
@@ -706,13 +706,13 @@
         <v>30.38</v>
       </c>
       <c r="C16" t="n">
-        <v>29.64636299647648</v>
+        <v>30.44348981295915</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.7336370035235191</v>
+        <v>0.06348981295915124</v>
       </c>
       <c r="E16" t="n">
-        <v>0.538223252938968</v>
+        <v>0.004030956349588008</v>
       </c>
     </row>
     <row r="17">
@@ -723,13 +723,13 @@
         <v>30.44</v>
       </c>
       <c r="C17" t="n">
-        <v>30.33773402865503</v>
+        <v>30.48743912317587</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.1022659713449734</v>
+        <v>0.04743912317586663</v>
       </c>
       <c r="E17" t="n">
-        <v>0.01045832889513092</v>
+        <v>0.002250470407695046</v>
       </c>
     </row>
     <row r="18">
@@ -740,13 +740,13 @@
         <v>30.48</v>
       </c>
       <c r="C18" t="n">
-        <v>30.36049336566984</v>
+        <v>30.45050122073281</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.1195066343301612</v>
+        <v>-0.02949877926718969</v>
       </c>
       <c r="E18" t="n">
-        <v>0.01428183564892286</v>
+        <v>0.0008701779782543803</v>
       </c>
     </row>
     <row r="19">
@@ -757,13 +757,13 @@
         <v>30.69</v>
       </c>
       <c r="C19" t="n">
-        <v>30.65505704903011</v>
+        <v>31.57859063932618</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.03494295096988864</v>
+        <v>0.8885906393261784</v>
       </c>
       <c r="E19" t="n">
-        <v>0.001221009822484041</v>
+        <v>0.7895933242981066</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +774,13 @@
         <v>30.75</v>
       </c>
       <c r="C20" t="n">
-        <v>30.32258370656307</v>
+        <v>30.82411957430374</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.4274162934369308</v>
+        <v>0.07411957430373661</v>
       </c>
       <c r="E20" t="n">
-        <v>0.1826846878953645</v>
+        <v>0.005493711294967132</v>
       </c>
     </row>
     <row r="21">
@@ -791,13 +791,13 @@
         <v>30.94</v>
       </c>
       <c r="C21" t="n">
-        <v>30.73581033191036</v>
+        <v>32.01803992955325</v>
       </c>
       <c r="D21" t="n">
-        <v>-0.2041896680896436</v>
+        <v>1.078039929553253</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0416934205545588</v>
+        <v>1.162170089711182</v>
       </c>
     </row>
     <row r="22">
@@ -808,13 +808,13 @@
         <v>30.95</v>
       </c>
       <c r="C22" t="n">
-        <v>31.06682419096773</v>
+        <v>31.06554974563931</v>
       </c>
       <c r="D22" t="n">
-        <v>0.1168241909677299</v>
+        <v>0.11554974563931</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01364789159526462</v>
+        <v>0.01335174371730923</v>
       </c>
     </row>
     <row r="23">
@@ -825,13 +825,13 @@
         <v>31.02</v>
       </c>
       <c r="C23" t="n">
-        <v>31.71203661379989</v>
+        <v>31.68144431219928</v>
       </c>
       <c r="D23" t="n">
-        <v>0.692036613799889</v>
+        <v>0.6614443121992757</v>
       </c>
       <c r="E23" t="n">
-        <v>0.4789146748396167</v>
+        <v>0.4375085781407729</v>
       </c>
     </row>
     <row r="24">
@@ -842,13 +842,13 @@
         <v>31.12</v>
       </c>
       <c r="C24" t="n">
-        <v>32.12226057527928</v>
+        <v>31.93836282950241</v>
       </c>
       <c r="D24" t="n">
-        <v>1.002260575279283</v>
+        <v>0.8183628295024086</v>
       </c>
       <c r="E24" t="n">
-        <v>1.00452626075916</v>
+        <v>0.6697177207111883</v>
       </c>
     </row>
     <row r="25">
@@ -859,13 +859,13 @@
         <v>31.28</v>
       </c>
       <c r="C25" t="n">
-        <v>32.26900250503424</v>
+        <v>32.68288845627483</v>
       </c>
       <c r="D25" t="n">
-        <v>0.989002505034243</v>
+        <v>1.40288845627483</v>
       </c>
       <c r="E25" t="n">
-        <v>0.9781259549640079</v>
+        <v>1.968096020749176</v>
       </c>
     </row>
     <row r="26">
@@ -876,13 +876,13 @@
         <v>31.38</v>
       </c>
       <c r="C26" t="n">
-        <v>32.11758947928325</v>
+        <v>31.92775612296992</v>
       </c>
       <c r="D26" t="n">
-        <v>0.7375894792832476</v>
+        <v>0.5477561229699184</v>
       </c>
       <c r="E26" t="n">
-        <v>0.5440382399493323</v>
+        <v>0.3000367702510364</v>
       </c>
     </row>
     <row r="27">
@@ -893,13 +893,13 @@
         <v>31.58</v>
       </c>
       <c r="C27" t="n">
-        <v>32.53827326168924</v>
+        <v>32.50689535741705</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9582732616892429</v>
+        <v>0.9268953574170524</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9182876440685401</v>
+        <v>0.8591350036012854</v>
       </c>
     </row>
     <row r="28">
@@ -910,13 +910,13 @@
         <v>31.65</v>
       </c>
       <c r="C28" t="n">
-        <v>32.52980955291806</v>
+        <v>31.6804080850526</v>
       </c>
       <c r="D28" t="n">
-        <v>0.8798095529180614</v>
+        <v>0.03040808505260628</v>
       </c>
       <c r="E28" t="n">
-        <v>0.7740648494058791</v>
+        <v>0.0009246516365665376</v>
       </c>
     </row>
     <row r="29">
@@ -927,13 +927,13 @@
         <v>31.88</v>
       </c>
       <c r="C29" t="n">
-        <v>33.277970159239</v>
+        <v>32.94701976420416</v>
       </c>
       <c r="D29" t="n">
-        <v>1.397970159238998</v>
+        <v>1.067019764204158</v>
       </c>
       <c r="E29" t="n">
-        <v>1.954320566122709</v>
+        <v>1.138531177202297</v>
       </c>
     </row>
     <row r="30">
@@ -944,13 +944,13 @@
         <v>32.28</v>
       </c>
       <c r="C30" t="n">
-        <v>32.85379537904976</v>
+        <v>33.16377948120398</v>
       </c>
       <c r="D30" t="n">
-        <v>0.5737953790497556</v>
+        <v>0.8837794812039803</v>
       </c>
       <c r="E30" t="n">
-        <v>0.3292411370188528</v>
+        <v>0.7810661713971766</v>
       </c>
     </row>
     <row r="31">
@@ -961,13 +961,13 @@
         <v>32.45</v>
       </c>
       <c r="C31" t="n">
-        <v>32.96916922584683</v>
+        <v>32.28287875391908</v>
       </c>
       <c r="D31" t="n">
-        <v>0.5191692258468237</v>
+        <v>-0.1671212460809244</v>
       </c>
       <c r="E31" t="n">
-        <v>0.2695366850663902</v>
+        <v>0.02792951089164088</v>
       </c>
     </row>
     <row r="32">
@@ -978,13 +978,13 @@
         <v>32.85</v>
       </c>
       <c r="C32" t="n">
-        <v>33.13367271978353</v>
+        <v>34.2162396324386</v>
       </c>
       <c r="D32" t="n">
-        <v>0.2836727197835245</v>
+        <v>1.366239632438599</v>
       </c>
       <c r="E32" t="n">
-        <v>0.080470211949382</v>
+        <v>1.866610733245959</v>
       </c>
     </row>
     <row r="33">
@@ -995,13 +995,13 @@
         <v>32.9</v>
       </c>
       <c r="C33" t="n">
-        <v>33.22534331497836</v>
+        <v>32.36611826104788</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3253433149783618</v>
+        <v>-0.5338817389521182</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1058482726011095</v>
+        <v>0.2850297111865377</v>
       </c>
     </row>
     <row r="34">
@@ -1012,13 +1012,13 @@
         <v>33.1</v>
       </c>
       <c r="C34" t="n">
-        <v>33.21840007594129</v>
+        <v>32.56279035552895</v>
       </c>
       <c r="D34" t="n">
-        <v>0.1184000759412882</v>
+        <v>-0.5372096444710479</v>
       </c>
       <c r="E34" t="n">
-        <v>0.01401857798290281</v>
+        <v>0.2885942021127097</v>
       </c>
     </row>
     <row r="35">
@@ -1029,13 +1029,13 @@
         <v>33.4</v>
       </c>
       <c r="C35" t="n">
-        <v>34.21330507641433</v>
+        <v>33.30642365044577</v>
       </c>
       <c r="D35" t="n">
-        <v>0.8133050764143306</v>
+        <v>-0.09357634955423322</v>
       </c>
       <c r="E35" t="n">
-        <v>0.6614651473213201</v>
+        <v>0.008756533195896043</v>
       </c>
     </row>
     <row r="36">
@@ -1046,13 +1046,13 @@
         <v>33.7</v>
       </c>
       <c r="C36" t="n">
-        <v>33.99777500965789</v>
+        <v>33.70611770471226</v>
       </c>
       <c r="D36" t="n">
-        <v>0.2977750096578902</v>
+        <v>0.006117704712252703</v>
       </c>
       <c r="E36" t="n">
-        <v>0.08866995637675658</v>
+        <v>3.742631094631893e-05</v>
       </c>
     </row>
     <row r="37">
@@ -1063,13 +1063,13 @@
         <v>34.1</v>
       </c>
       <c r="C37" t="n">
-        <v>34.04644958257992</v>
+        <v>34.61605223088247</v>
       </c>
       <c r="D37" t="n">
-        <v>-0.05355041742008382</v>
+        <v>0.5160522308824653</v>
       </c>
       <c r="E37" t="n">
-        <v>0.002867647205865216</v>
+        <v>0.2663099049987693</v>
       </c>
     </row>
     <row r="38">
@@ -1080,13 +1080,13 @@
         <v>34.4</v>
       </c>
       <c r="C38" t="n">
-        <v>34.57601968097843</v>
+        <v>34.31129008754729</v>
       </c>
       <c r="D38" t="n">
-        <v>0.1760196809784276</v>
+        <v>-0.08870991245270687</v>
       </c>
       <c r="E38" t="n">
-        <v>0.03098292809174742</v>
+        <v>0.007869448567366918</v>
       </c>
     </row>
     <row r="39">
@@ -1097,13 +1097,13 @@
         <v>34.9</v>
       </c>
       <c r="C39" t="n">
-        <v>34.85083618170182</v>
+        <v>35.30499002121963</v>
       </c>
       <c r="D39" t="n">
-        <v>-0.04916381829818306</v>
+        <v>0.404990021219632</v>
       </c>
       <c r="E39" t="n">
-        <v>0.002417081029656759</v>
+        <v>0.164016917287478</v>
       </c>
     </row>
     <row r="40">
@@ -1114,13 +1114,13 @@
         <v>35.3</v>
       </c>
       <c r="C40" t="n">
-        <v>35.9687543924692</v>
+        <v>35.10723594525111</v>
       </c>
       <c r="D40" t="n">
-        <v>0.6687543924692037</v>
+        <v>-0.1927640547488849</v>
       </c>
       <c r="E40" t="n">
-        <v>0.4472324374468536</v>
+        <v>0.0371579808032311</v>
       </c>
     </row>
     <row r="41">
@@ -1131,13 +1131,13 @@
         <v>35.7</v>
       </c>
       <c r="C41" t="n">
-        <v>36.10000759518975</v>
+        <v>35.6412975690336</v>
       </c>
       <c r="D41" t="n">
-        <v>0.4000075951897486</v>
+        <v>-0.05870243096639882</v>
       </c>
       <c r="E41" t="n">
-        <v>0.1600060762094858</v>
+        <v>0.003445975401364819</v>
       </c>
     </row>
     <row r="42">
@@ -1148,13 +1148,13 @@
         <v>36.3</v>
       </c>
       <c r="C42" t="n">
-        <v>35.91907778380174</v>
+        <v>36.21455944135352</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.3809222161982575</v>
+        <v>-0.08544055864648215</v>
       </c>
       <c r="E42" t="n">
-        <v>0.145101734793392</v>
+        <v>0.007300089061822955</v>
       </c>
     </row>
     <row r="43">
@@ -1165,13 +1165,13 @@
         <v>36.8</v>
       </c>
       <c r="C43" t="n">
-        <v>36.40238053655096</v>
+        <v>36.49702268034099</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.3976194634490327</v>
+        <v>-0.3029773196590071</v>
       </c>
       <c r="E43" t="n">
-        <v>0.1581012377134966</v>
+        <v>0.09179525622775617</v>
       </c>
     </row>
     <row r="44">
@@ -1182,13 +1182,13 @@
         <v>37.3</v>
       </c>
       <c r="C44" t="n">
-        <v>36.34026366487587</v>
+        <v>37.20155162870451</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.959736335124127</v>
+        <v>-0.09844837129548267</v>
       </c>
       <c r="E44" t="n">
-        <v>0.9210938329574907</v>
+        <v>0.009692081810733217</v>
       </c>
     </row>
     <row r="45">
@@ -1199,13 +1199,13 @@
         <v>37.9</v>
       </c>
       <c r="C45" t="n">
-        <v>37.45542092048556</v>
+        <v>39.15502187870906</v>
       </c>
       <c r="D45" t="n">
-        <v>-0.4445790795144404</v>
+        <v>1.255021878709059</v>
       </c>
       <c r="E45" t="n">
-        <v>0.1976505579419071</v>
+        <v>1.575079916038415</v>
       </c>
     </row>
     <row r="46">
@@ -1216,13 +1216,13 @@
         <v>38.5</v>
       </c>
       <c r="C46" t="n">
-        <v>38.17963449233827</v>
+        <v>39.24086098913765</v>
       </c>
       <c r="D46" t="n">
-        <v>-0.3203655076617338</v>
+        <v>0.7408609891376514</v>
       </c>
       <c r="E46" t="n">
-        <v>0.1026340584993604</v>
+        <v>0.5488750052260193</v>
       </c>
     </row>
     <row r="47">
@@ -1233,13 +1233,13 @@
         <v>38.9</v>
       </c>
       <c r="C47" t="n">
-        <v>38.58431861107851</v>
+        <v>39.07086653964407</v>
       </c>
       <c r="D47" t="n">
-        <v>-0.3156813889214902</v>
+        <v>0.1708665396440736</v>
       </c>
       <c r="E47" t="n">
-        <v>0.09965473931140117</v>
+        <v>0.02919537436993978</v>
       </c>
     </row>
     <row r="48">
@@ -1250,13 +1250,13 @@
         <v>39.4</v>
       </c>
       <c r="C48" t="n">
-        <v>38.90683823342697</v>
+        <v>39.51592348560242</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.4931617665730244</v>
+        <v>0.1159234856024227</v>
       </c>
       <c r="E48" t="n">
-        <v>0.2432085280094262</v>
+        <v>0.01343825451421511</v>
       </c>
     </row>
     <row r="49">
@@ -1267,13 +1267,13 @@
         <v>39.9</v>
       </c>
       <c r="C49" t="n">
-        <v>39.41233102678765</v>
+        <v>40.580271733598</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.4876689732123509</v>
+        <v>0.6802717335979978</v>
       </c>
       <c r="E49" t="n">
-        <v>0.2378210274339886</v>
+        <v>0.4627696315324252</v>
       </c>
     </row>
     <row r="50">
@@ -1284,13 +1284,13 @@
         <v>40.1</v>
       </c>
       <c r="C50" t="n">
-        <v>39.24870500583931</v>
+        <v>36.69296421120788</v>
       </c>
       <c r="D50" t="n">
-        <v>-0.8512949941606962</v>
+        <v>-3.407035788792122</v>
       </c>
       <c r="E50" t="n">
-        <v>0.7247031670830598</v>
+        <v>11.60789286611036</v>
       </c>
     </row>
     <row r="51">
@@ -1301,13 +1301,13 @@
         <v>40.6</v>
       </c>
       <c r="C51" t="n">
-        <v>39.33456577636483</v>
+        <v>39.81737960129512</v>
       </c>
       <c r="D51" t="n">
-        <v>-1.265434223635175</v>
+        <v>-0.7826203987048785</v>
       </c>
       <c r="E51" t="n">
-        <v>1.601323774347159</v>
+        <v>0.612494688468983</v>
       </c>
     </row>
     <row r="52">
@@ -1318,11 +1318,11 @@
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="n">
-        <v>-0.008685308628653132</v>
+        <v>5.158801916162126</v>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>18.1450358373095</v>
+        <v>32.9098687657843</v>
       </c>
     </row>
     <row r="53">
@@ -1335,7 +1335,7 @@
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>0.36290071674619</v>
+        <v>0.658197375315686</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add weight setting method, implement additional activation functions, and enhance gradient descent optimizer
</commit_message>
<xml_diff>
--- a/full/sliding_window_results_window_1.xlsx
+++ b/full/sliding_window_results_window_1.xlsx
@@ -468,13 +468,13 @@
         <v>28.98</v>
       </c>
       <c r="C2" t="n">
-        <v>28.79420114517954</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1857988548204652</v>
+        <v>-28.98</v>
       </c>
       <c r="E2" t="n">
-        <v>0.03452121445259631</v>
+        <v>839.8404</v>
       </c>
     </row>
     <row r="3">
@@ -485,13 +485,13 @@
         <v>29.15</v>
       </c>
       <c r="C3" t="n">
-        <v>26.8952755278337</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>-2.254724472166298</v>
+        <v>-29.15</v>
       </c>
       <c r="E3" t="n">
-        <v>5.083782445385594</v>
+        <v>849.7225</v>
       </c>
     </row>
     <row r="4">
@@ -502,13 +502,13 @@
         <v>29.35</v>
       </c>
       <c r="C4" t="n">
-        <v>28.3277035906885</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>-1.022296409311505</v>
+        <v>-29.35</v>
       </c>
       <c r="E4" t="n">
-        <v>1.045089948491195</v>
+        <v>861.4225000000001</v>
       </c>
     </row>
     <row r="5">
@@ -519,13 +519,13 @@
         <v>29.37</v>
       </c>
       <c r="C5" t="n">
-        <v>28.97599378585091</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.3940062141490905</v>
+        <v>-29.37</v>
       </c>
       <c r="E5" t="n">
-        <v>0.155240896788099</v>
+        <v>862.5969</v>
       </c>
     </row>
     <row r="6">
@@ -536,13 +536,13 @@
         <v>29.54</v>
       </c>
       <c r="C6" t="n">
-        <v>28.44247481655044</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>-1.097525183449562</v>
+        <v>-29.54</v>
       </c>
       <c r="E6" t="n">
-        <v>1.204561528305995</v>
+        <v>872.6116</v>
       </c>
     </row>
     <row r="7">
@@ -553,13 +553,13 @@
         <v>29.55</v>
       </c>
       <c r="C7" t="n">
-        <v>27.43885991441575</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-2.11114008558425</v>
+        <v>-29.55</v>
       </c>
       <c r="E7" t="n">
-        <v>4.456912460960673</v>
+        <v>873.2025</v>
       </c>
     </row>
     <row r="8">
@@ -570,13 +570,13 @@
         <v>29.75</v>
       </c>
       <c r="C8" t="n">
-        <v>28.75116319177424</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.9988368082257573</v>
+        <v>-29.75</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9976749694666182</v>
+        <v>885.0625</v>
       </c>
     </row>
     <row r="9">
@@ -587,13 +587,13 @@
         <v>29.84</v>
       </c>
       <c r="C9" t="n">
-        <v>29.62522956125434</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.2147704387456635</v>
+        <v>-29.84</v>
       </c>
       <c r="E9" t="n">
-        <v>0.04612634135900479</v>
+        <v>890.4256</v>
       </c>
     </row>
     <row r="10">
@@ -604,13 +604,13 @@
         <v>29.81</v>
       </c>
       <c r="C10" t="n">
-        <v>30.33137008970033</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0.5213700897003299</v>
+        <v>-29.81</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2718267704341301</v>
+        <v>888.6360999999999</v>
       </c>
     </row>
     <row r="11">
@@ -621,13 +621,13 @@
         <v>29.92</v>
       </c>
       <c r="C11" t="n">
-        <v>31.23216812480042</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>1.312168124800422</v>
+        <v>-29.92</v>
       </c>
       <c r="E11" t="n">
-        <v>1.721785187742257</v>
+        <v>895.2064000000001</v>
       </c>
     </row>
     <row r="12">
@@ -638,13 +638,13 @@
         <v>29.98</v>
       </c>
       <c r="C12" t="n">
-        <v>30.70641612268779</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.726416122687791</v>
+        <v>-29.98</v>
       </c>
       <c r="E12" t="n">
-        <v>0.5276803833007638</v>
+        <v>898.8004000000001</v>
       </c>
     </row>
     <row r="13">
@@ -655,13 +655,13 @@
         <v>30.04</v>
       </c>
       <c r="C13" t="n">
-        <v>30.19832853473281</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>0.1583285347328136</v>
+        <v>-30.04</v>
       </c>
       <c r="E13" t="n">
-        <v>0.02506792491063977</v>
+        <v>902.4015999999999</v>
       </c>
     </row>
     <row r="14">
@@ -672,13 +672,13 @@
         <v>30.21</v>
       </c>
       <c r="C14" t="n">
-        <v>29.74811100658376</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-0.4618889934162453</v>
+        <v>-30.21</v>
       </c>
       <c r="E14" t="n">
-        <v>0.2133414422390723</v>
+        <v>912.6441000000001</v>
       </c>
     </row>
     <row r="15">
@@ -689,13 +689,13 @@
         <v>30.22</v>
       </c>
       <c r="C15" t="n">
-        <v>29.27235730146522</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.9476426985347821</v>
+        <v>-30.22</v>
       </c>
       <c r="E15" t="n">
-        <v>0.8980266840862839</v>
+        <v>913.2483999999999</v>
       </c>
     </row>
     <row r="16">
@@ -706,13 +706,13 @@
         <v>30.38</v>
       </c>
       <c r="C16" t="n">
-        <v>30.12718722773184</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.252812772268161</v>
+        <v>-30.38</v>
       </c>
       <c r="E16" t="n">
-        <v>0.06391429782191305</v>
+        <v>922.9444</v>
       </c>
     </row>
     <row r="17">
@@ -723,13 +723,13 @@
         <v>30.44</v>
       </c>
       <c r="C17" t="n">
-        <v>29.86411394993171</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-0.5758860500682914</v>
+        <v>-30.44</v>
       </c>
       <c r="E17" t="n">
-        <v>0.3316447426632587</v>
+        <v>926.5936</v>
       </c>
     </row>
     <row r="18">
@@ -740,13 +740,13 @@
         <v>30.48</v>
       </c>
       <c r="C18" t="n">
-        <v>30.623051629318</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>0.1430516293179949</v>
+        <v>-30.48</v>
       </c>
       <c r="E18" t="n">
-        <v>0.02046376865053301</v>
+        <v>929.0304</v>
       </c>
     </row>
     <row r="19">
@@ -757,13 +757,13 @@
         <v>30.69</v>
       </c>
       <c r="C19" t="n">
-        <v>31.58582675266142</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>0.8958267526614172</v>
+        <v>-30.69</v>
       </c>
       <c r="E19" t="n">
-        <v>0.8025055707838999</v>
+        <v>941.8761000000001</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +774,13 @@
         <v>30.75</v>
       </c>
       <c r="C20" t="n">
-        <v>30.86780570249843</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>0.1178057024984334</v>
+        <v>-30.75</v>
       </c>
       <c r="E20" t="n">
-        <v>0.01387818354114939</v>
+        <v>945.5625</v>
       </c>
     </row>
     <row r="21">
@@ -791,13 +791,13 @@
         <v>30.94</v>
       </c>
       <c r="C21" t="n">
-        <v>32.06882924787063</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>1.12882924787063</v>
+        <v>-30.94</v>
       </c>
       <c r="E21" t="n">
-        <v>1.274255470848173</v>
+        <v>957.2836000000001</v>
       </c>
     </row>
     <row r="22">
@@ -808,13 +808,13 @@
         <v>30.95</v>
       </c>
       <c r="C22" t="n">
-        <v>31.60162178139203</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6516217813920306</v>
+        <v>-30.95</v>
       </c>
       <c r="E22" t="n">
-        <v>0.4246109459845234</v>
+        <v>957.9024999999999</v>
       </c>
     </row>
     <row r="23">
@@ -825,13 +825,13 @@
         <v>31.02</v>
       </c>
       <c r="C23" t="n">
-        <v>31.57240520523766</v>
+        <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>0.5524052052376618</v>
+        <v>-31.02</v>
       </c>
       <c r="E23" t="n">
-        <v>0.3051515107736633</v>
+        <v>962.2404</v>
       </c>
     </row>
     <row r="24">
@@ -842,13 +842,13 @@
         <v>31.12</v>
       </c>
       <c r="C24" t="n">
-        <v>31.63832335387873</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0.5183233538787242</v>
+        <v>-31.12</v>
       </c>
       <c r="E24" t="n">
-        <v>0.2686590991760892</v>
+        <v>968.4544000000001</v>
       </c>
     </row>
     <row r="25">
@@ -859,13 +859,13 @@
         <v>31.28</v>
       </c>
       <c r="C25" t="n">
-        <v>32.30159313130456</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>1.021593131304563</v>
+        <v>-31.28</v>
       </c>
       <c r="E25" t="n">
-        <v>1.043652525928662</v>
+        <v>978.4384000000001</v>
       </c>
     </row>
     <row r="26">
@@ -876,13 +876,13 @@
         <v>31.38</v>
       </c>
       <c r="C26" t="n">
-        <v>32.27579443633687</v>
+        <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>0.8957944363368675</v>
+        <v>-31.38</v>
       </c>
       <c r="E26" t="n">
-        <v>0.8024476721720861</v>
+        <v>984.7044</v>
       </c>
     </row>
     <row r="27">
@@ -893,13 +893,13 @@
         <v>31.58</v>
       </c>
       <c r="C27" t="n">
-        <v>32.53275266783223</v>
+        <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>0.9527526678322289</v>
+        <v>-31.58</v>
       </c>
       <c r="E27" t="n">
-        <v>0.9077376460614295</v>
+        <v>997.2963999999999</v>
       </c>
     </row>
     <row r="28">
@@ -910,13 +910,13 @@
         <v>31.65</v>
       </c>
       <c r="C28" t="n">
-        <v>31.63595667675154</v>
+        <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-0.0140433232484547</v>
+        <v>-31.65</v>
       </c>
       <c r="E28" t="n">
-        <v>0.0001972149278605882</v>
+        <v>1001.7225</v>
       </c>
     </row>
     <row r="29">
@@ -927,13 +927,13 @@
         <v>31.88</v>
       </c>
       <c r="C29" t="n">
-        <v>32.30768536830329</v>
+        <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>0.4276853683032904</v>
+        <v>-31.88</v>
       </c>
       <c r="E29" t="n">
-        <v>0.1829147742607212</v>
+        <v>1016.3344</v>
       </c>
     </row>
     <row r="30">
@@ -944,13 +944,13 @@
         <v>32.28</v>
       </c>
       <c r="C30" t="n">
-        <v>32.90671252937075</v>
+        <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>0.6267125293707494</v>
+        <v>-32.28</v>
       </c>
       <c r="E30" t="n">
-        <v>0.3927685944702824</v>
+        <v>1041.9984</v>
       </c>
     </row>
     <row r="31">
@@ -961,13 +961,13 @@
         <v>32.45</v>
       </c>
       <c r="C31" t="n">
-        <v>31.97511605218969</v>
+        <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-0.4748839478103157</v>
+        <v>-32.45</v>
       </c>
       <c r="E31" t="n">
-        <v>0.2255147638879107</v>
+        <v>1053.0025</v>
       </c>
     </row>
     <row r="32">
@@ -978,13 +978,13 @@
         <v>32.85</v>
       </c>
       <c r="C32" t="n">
-        <v>33.70458996877836</v>
+        <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>0.854589968778356</v>
+        <v>-32.85</v>
       </c>
       <c r="E32" t="n">
-        <v>0.7303240147365915</v>
+        <v>1079.1225</v>
       </c>
     </row>
     <row r="33">
@@ -995,13 +995,13 @@
         <v>32.9</v>
       </c>
       <c r="C33" t="n">
-        <v>33.26892404408035</v>
+        <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>0.3689240440803516</v>
+        <v>-32.9</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1361049503006012</v>
+        <v>1082.41</v>
       </c>
     </row>
     <row r="34">
@@ -1012,13 +1012,13 @@
         <v>33.1</v>
       </c>
       <c r="C34" t="n">
-        <v>32.47785729315988</v>
+        <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>-0.6221427068401226</v>
+        <v>-33.1</v>
       </c>
       <c r="E34" t="n">
-        <v>0.3870615476743547</v>
+        <v>1095.61</v>
       </c>
     </row>
     <row r="35">
@@ -1029,13 +1029,13 @@
         <v>33.4</v>
       </c>
       <c r="C35" t="n">
-        <v>32.47542346711217</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>-0.9245765328878264</v>
+        <v>-33.4</v>
       </c>
       <c r="E35" t="n">
-        <v>0.8548417651668739</v>
+        <v>1115.56</v>
       </c>
     </row>
     <row r="36">
@@ -1046,13 +1046,13 @@
         <v>33.7</v>
       </c>
       <c r="C36" t="n">
-        <v>33.22482490097976</v>
+        <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>-0.475175099020241</v>
+        <v>-33.7</v>
       </c>
       <c r="E36" t="n">
-        <v>0.2257913747288958</v>
+        <v>1135.69</v>
       </c>
     </row>
     <row r="37">
@@ -1063,13 +1063,13 @@
         <v>34.1</v>
       </c>
       <c r="C37" t="n">
-        <v>34.25024351619407</v>
+        <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>0.1502435161940667</v>
+        <v>-34.1</v>
       </c>
       <c r="E37" t="n">
-        <v>0.02257311415835679</v>
+        <v>1162.81</v>
       </c>
     </row>
     <row r="38">
@@ -1080,13 +1080,13 @@
         <v>34.4</v>
       </c>
       <c r="C38" t="n">
-        <v>34.22570711600993</v>
+        <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>-0.1742928839900699</v>
+        <v>-34.4</v>
       </c>
       <c r="E38" t="n">
-        <v>0.03037800940957597</v>
+        <v>1183.36</v>
       </c>
     </row>
     <row r="39">
@@ -1097,13 +1097,13 @@
         <v>34.9</v>
       </c>
       <c r="C39" t="n">
-        <v>34.94756014124237</v>
+        <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0475601412423714</v>
+        <v>-34.9</v>
       </c>
       <c r="E39" t="n">
-        <v>0.002261967034994317</v>
+        <v>1218.01</v>
       </c>
     </row>
     <row r="40">
@@ -1114,13 +1114,13 @@
         <v>35.3</v>
       </c>
       <c r="C40" t="n">
-        <v>34.55623597867603</v>
+        <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>-0.7437640213239689</v>
+        <v>-35.3</v>
       </c>
       <c r="E40" t="n">
-        <v>0.5531849194160012</v>
+        <v>1246.09</v>
       </c>
     </row>
     <row r="41">
@@ -1131,13 +1131,13 @@
         <v>35.7</v>
       </c>
       <c r="C41" t="n">
-        <v>35.09183405652182</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>-0.6081659434781841</v>
+        <v>-35.7</v>
       </c>
       <c r="E41" t="n">
-        <v>0.3698658148067098</v>
+        <v>1274.49</v>
       </c>
     </row>
     <row r="42">
@@ -1148,13 +1148,13 @@
         <v>36.3</v>
       </c>
       <c r="C42" t="n">
-        <v>35.80248031508984</v>
+        <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>-0.4975196849101593</v>
+        <v>-36.3</v>
       </c>
       <c r="E42" t="n">
-        <v>0.2475258368731042</v>
+        <v>1317.69</v>
       </c>
     </row>
     <row r="43">
@@ -1165,13 +1165,13 @@
         <v>36.8</v>
       </c>
       <c r="C43" t="n">
-        <v>36.17637596632949</v>
+        <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>-0.6236240336705094</v>
+        <v>-36.8</v>
       </c>
       <c r="E43" t="n">
-        <v>0.3889069353714767</v>
+        <v>1354.24</v>
       </c>
     </row>
     <row r="44">
@@ -1182,13 +1182,13 @@
         <v>37.3</v>
       </c>
       <c r="C44" t="n">
-        <v>37.2042008037133</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>-0.09579919628669842</v>
+        <v>-37.3</v>
       </c>
       <c r="E44" t="n">
-        <v>0.009177486009177373</v>
+        <v>1391.29</v>
       </c>
     </row>
     <row r="45">
@@ -1199,13 +1199,13 @@
         <v>37.9</v>
       </c>
       <c r="C45" t="n">
-        <v>38.4487096805945</v>
+        <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>0.5487096805945058</v>
+        <v>-37.9</v>
       </c>
       <c r="E45" t="n">
-        <v>0.3010823135781245</v>
+        <v>1436.41</v>
       </c>
     </row>
     <row r="46">
@@ -1216,13 +1216,13 @@
         <v>38.5</v>
       </c>
       <c r="C46" t="n">
-        <v>38.50592315034655</v>
+        <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>0.00592315034654689</v>
+        <v>-38.5</v>
       </c>
       <c r="E46" t="n">
-        <v>3.508371002779855e-05</v>
+        <v>1482.25</v>
       </c>
     </row>
     <row r="47">
@@ -1233,13 +1233,13 @@
         <v>38.9</v>
       </c>
       <c r="C47" t="n">
-        <v>38.90395655176361</v>
+        <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>0.003956551763607763</v>
+        <v>-38.9</v>
       </c>
       <c r="E47" t="n">
-        <v>1.56543018581077e-05</v>
+        <v>1513.21</v>
       </c>
     </row>
     <row r="48">
@@ -1250,13 +1250,13 @@
         <v>39.4</v>
       </c>
       <c r="C48" t="n">
-        <v>39.39414069587665</v>
+        <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>-0.005859304123347897</v>
+        <v>-39.4</v>
       </c>
       <c r="E48" t="n">
-        <v>3.433144480988167e-05</v>
+        <v>1552.36</v>
       </c>
     </row>
     <row r="49">
@@ -1267,13 +1267,13 @@
         <v>39.9</v>
       </c>
       <c r="C49" t="n">
-        <v>39.41557131146828</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>-0.4844286885317146</v>
+        <v>-39.9</v>
       </c>
       <c r="E49" t="n">
-        <v>0.234671154272557</v>
+        <v>1592.01</v>
       </c>
     </row>
     <row r="50">
@@ -1284,13 +1284,13 @@
         <v>40.1</v>
       </c>
       <c r="C50" t="n">
-        <v>37.65003583774943</v>
+        <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>-2.449964162250573</v>
+        <v>-40.1</v>
       </c>
       <c r="E50" t="n">
-        <v>6.002324396312154</v>
+        <v>1608.01</v>
       </c>
     </row>
     <row r="51">
@@ -1301,13 +1301,13 @@
         <v>40.6</v>
       </c>
       <c r="C51" t="n">
-        <v>39.73876186553645</v>
+        <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>-0.8612381344635551</v>
+        <v>-40.6</v>
       </c>
       <c r="E51" t="n">
-        <v>0.7417311242542647</v>
+        <v>1648.36</v>
       </c>
     </row>
     <row r="52">
@@ -1318,11 +1318,11 @@
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="n">
-        <v>-6.942214912650059</v>
+        <v>-1641.03</v>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>34.97984677343559</v>
+        <v>54420.1889</v>
       </c>
     </row>
     <row r="53">
@@ -1335,7 +1335,7 @@
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>0.6995969354687118</v>
+        <v>1088.403778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor weight handling methods in DenseLayer and NeuralNetwork
</commit_message>
<xml_diff>
--- a/full/sliding_window_results_window_1.xlsx
+++ b/full/sliding_window_results_window_1.xlsx
@@ -468,13 +468,13 @@
         <v>28.98</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>29.72175776911019</v>
       </c>
       <c r="D2" t="n">
-        <v>-28.98</v>
+        <v>0.7417577691101904</v>
       </c>
       <c r="E2" t="n">
-        <v>839.8404</v>
+        <v>0.5502045880353266</v>
       </c>
     </row>
     <row r="3">
@@ -485,13 +485,13 @@
         <v>29.15</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>30.02891384579398</v>
       </c>
       <c r="D3" t="n">
-        <v>-29.15</v>
+        <v>0.8789138457939778</v>
       </c>
       <c r="E3" t="n">
-        <v>849.7225</v>
+        <v>0.7724895483283601</v>
       </c>
     </row>
     <row r="4">
@@ -502,13 +502,13 @@
         <v>29.35</v>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>29.87532757460375</v>
       </c>
       <c r="D4" t="n">
-        <v>-29.35</v>
+        <v>0.5253275746037467</v>
       </c>
       <c r="E4" t="n">
-        <v>861.4225000000001</v>
+        <v>0.275969060639055</v>
       </c>
     </row>
     <row r="5">
@@ -519,13 +519,13 @@
         <v>29.37</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>29.64943781981881</v>
       </c>
       <c r="D5" t="n">
-        <v>-29.37</v>
+        <v>0.2794378198188099</v>
       </c>
       <c r="E5" t="n">
-        <v>862.5969</v>
+        <v>0.07808549514508965</v>
       </c>
     </row>
     <row r="6">
@@ -536,13 +536,13 @@
         <v>29.54</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>30.2197193266033</v>
       </c>
       <c r="D6" t="n">
-        <v>-29.54</v>
+        <v>0.6797193266032977</v>
       </c>
       <c r="E6" t="n">
-        <v>872.6116</v>
+        <v>0.4620183629580405</v>
       </c>
     </row>
     <row r="7">
@@ -553,13 +553,13 @@
         <v>29.55</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>30.16524852836157</v>
       </c>
       <c r="D7" t="n">
-        <v>-29.55</v>
+        <v>0.6152485283615654</v>
       </c>
       <c r="E7" t="n">
-        <v>873.2025</v>
+        <v>0.378530751651072</v>
       </c>
     </row>
     <row r="8">
@@ -570,13 +570,13 @@
         <v>29.75</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>30.95421275670812</v>
       </c>
       <c r="D8" t="n">
-        <v>-29.75</v>
+        <v>1.20421275670812</v>
       </c>
       <c r="E8" t="n">
-        <v>885.0625</v>
+        <v>1.45012836341857</v>
       </c>
     </row>
     <row r="9">
@@ -587,13 +587,13 @@
         <v>29.84</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>30.3238393500008</v>
       </c>
       <c r="D9" t="n">
-        <v>-29.84</v>
+        <v>0.483839350000796</v>
       </c>
       <c r="E9" t="n">
-        <v>890.4256</v>
+        <v>0.2341005166091928</v>
       </c>
     </row>
     <row r="10">
@@ -604,13 +604,13 @@
         <v>29.81</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>29.46879379716013</v>
       </c>
       <c r="D10" t="n">
-        <v>-29.81</v>
+        <v>-0.3412062028398708</v>
       </c>
       <c r="E10" t="n">
-        <v>888.6360999999999</v>
+        <v>0.116421672856403</v>
       </c>
     </row>
     <row r="11">
@@ -621,13 +621,13 @@
         <v>29.92</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>30.68162427992516</v>
       </c>
       <c r="D11" t="n">
-        <v>-29.92</v>
+        <v>0.761624279925158</v>
       </c>
       <c r="E11" t="n">
-        <v>895.2064000000001</v>
+        <v>0.5800715437715155</v>
       </c>
     </row>
     <row r="12">
@@ -638,13 +638,13 @@
         <v>29.98</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>30.02526259058906</v>
       </c>
       <c r="D12" t="n">
-        <v>-29.98</v>
+        <v>0.04526259058906135</v>
       </c>
       <c r="E12" t="n">
-        <v>898.8004000000001</v>
+        <v>0.002048702106832985</v>
       </c>
     </row>
     <row r="13">
@@ -655,13 +655,13 @@
         <v>30.04</v>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>29.65885848788355</v>
       </c>
       <c r="D13" t="n">
-        <v>-30.04</v>
+        <v>-0.3811415121164501</v>
       </c>
       <c r="E13" t="n">
-        <v>902.4015999999999</v>
+        <v>0.1452688522584141</v>
       </c>
     </row>
     <row r="14">
@@ -672,13 +672,13 @@
         <v>30.21</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>30.0738608790388</v>
       </c>
       <c r="D14" t="n">
-        <v>-30.21</v>
+        <v>-0.1361391209612037</v>
       </c>
       <c r="E14" t="n">
-        <v>912.6441000000001</v>
+        <v>0.01853386025608926</v>
       </c>
     </row>
     <row r="15">
@@ -689,13 +689,13 @@
         <v>30.22</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>29.9260358867717</v>
       </c>
       <c r="D15" t="n">
-        <v>-30.22</v>
+        <v>-0.2939641132282951</v>
       </c>
       <c r="E15" t="n">
-        <v>913.2483999999999</v>
+        <v>0.08641489986609789</v>
       </c>
     </row>
     <row r="16">
@@ -706,13 +706,13 @@
         <v>30.38</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>29.94177716779699</v>
       </c>
       <c r="D16" t="n">
-        <v>-30.38</v>
+        <v>-0.4382228322030066</v>
       </c>
       <c r="E16" t="n">
-        <v>922.9444</v>
+        <v>0.1920392506640245</v>
       </c>
     </row>
     <row r="17">
@@ -723,13 +723,13 @@
         <v>30.44</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>29.90366860471718</v>
       </c>
       <c r="D17" t="n">
-        <v>-30.44</v>
+        <v>-0.5363313952828221</v>
       </c>
       <c r="E17" t="n">
-        <v>926.5936</v>
+        <v>0.2876513655660188</v>
       </c>
     </row>
     <row r="18">
@@ -740,13 +740,13 @@
         <v>30.48</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>29.86792644700605</v>
       </c>
       <c r="D18" t="n">
-        <v>-30.48</v>
+        <v>-0.6120735529939552</v>
       </c>
       <c r="E18" t="n">
-        <v>929.0304</v>
+        <v>0.374634034274644</v>
       </c>
     </row>
     <row r="19">
@@ -757,13 +757,13 @@
         <v>30.69</v>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>30.78666544642995</v>
       </c>
       <c r="D19" t="n">
-        <v>-30.69</v>
+        <v>0.09666544642994523</v>
       </c>
       <c r="E19" t="n">
-        <v>941.8761000000001</v>
+        <v>0.009344208533500611</v>
       </c>
     </row>
     <row r="20">
@@ -774,13 +774,13 @@
         <v>30.75</v>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>30.99431524769091</v>
       </c>
       <c r="D20" t="n">
-        <v>-30.75</v>
+        <v>0.2443152476909134</v>
       </c>
       <c r="E20" t="n">
-        <v>945.5625</v>
+        <v>0.05968994025427236</v>
       </c>
     </row>
     <row r="21">
@@ -791,13 +791,13 @@
         <v>30.94</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>31.60933116519394</v>
       </c>
       <c r="D21" t="n">
-        <v>-30.94</v>
+        <v>0.6693311651939347</v>
       </c>
       <c r="E21" t="n">
-        <v>957.2836000000001</v>
+        <v>0.4480042086998702</v>
       </c>
     </row>
     <row r="22">
@@ -808,13 +808,13 @@
         <v>30.95</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>31.35647702173609</v>
       </c>
       <c r="D22" t="n">
-        <v>-30.95</v>
+        <v>0.4064770217360909</v>
       </c>
       <c r="E22" t="n">
-        <v>957.9024999999999</v>
+        <v>0.1652235691994425</v>
       </c>
     </row>
     <row r="23">
@@ -825,13 +825,13 @@
         <v>31.02</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>31.14129646547685</v>
       </c>
       <c r="D23" t="n">
-        <v>-31.02</v>
+        <v>0.1212964654768527</v>
       </c>
       <c r="E23" t="n">
-        <v>962.2404</v>
+        <v>0.01471283253717732</v>
       </c>
     </row>
     <row r="24">
@@ -842,13 +842,13 @@
         <v>31.12</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>31.11198262567547</v>
       </c>
       <c r="D24" t="n">
-        <v>-31.12</v>
+        <v>-0.008017374324534643</v>
       </c>
       <c r="E24" t="n">
-        <v>968.4544000000001</v>
+        <v>6.427829105970732e-05</v>
       </c>
     </row>
     <row r="25">
@@ -859,13 +859,13 @@
         <v>31.28</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>31.61760285234385</v>
       </c>
       <c r="D25" t="n">
-        <v>-31.28</v>
+        <v>0.3376028523438528</v>
       </c>
       <c r="E25" t="n">
-        <v>978.4384000000001</v>
+        <v>0.1139756859107053</v>
       </c>
     </row>
     <row r="26">
@@ -876,13 +876,13 @@
         <v>31.38</v>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>31.5746255466973</v>
       </c>
       <c r="D26" t="n">
-        <v>-31.38</v>
+        <v>0.1946255466973028</v>
       </c>
       <c r="E26" t="n">
-        <v>984.7044</v>
+        <v>0.037879103427224</v>
       </c>
     </row>
     <row r="27">
@@ -893,13 +893,13 @@
         <v>31.58</v>
       </c>
       <c r="C27" t="n">
-        <v>0</v>
+        <v>31.46276909702048</v>
       </c>
       <c r="D27" t="n">
-        <v>-31.58</v>
+        <v>-0.117230902979518</v>
       </c>
       <c r="E27" t="n">
-        <v>997.2963999999999</v>
+        <v>0.01374308461339316</v>
       </c>
     </row>
     <row r="28">
@@ -910,13 +910,13 @@
         <v>31.65</v>
       </c>
       <c r="C28" t="n">
-        <v>0</v>
+        <v>31.6124046137601</v>
       </c>
       <c r="D28" t="n">
-        <v>-31.65</v>
+        <v>-0.03759538623989656</v>
       </c>
       <c r="E28" t="n">
-        <v>1001.7225</v>
+        <v>0.001413413066527003</v>
       </c>
     </row>
     <row r="29">
@@ -927,13 +927,13 @@
         <v>31.88</v>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>32.07227687734462</v>
       </c>
       <c r="D29" t="n">
-        <v>-31.88</v>
+        <v>0.1922768773446215</v>
       </c>
       <c r="E29" t="n">
-        <v>1016.3344</v>
+        <v>0.03697039756139862</v>
       </c>
     </row>
     <row r="30">
@@ -944,13 +944,13 @@
         <v>32.28</v>
       </c>
       <c r="C30" t="n">
-        <v>0</v>
+        <v>32.43597484441806</v>
       </c>
       <c r="D30" t="n">
-        <v>-32.28</v>
+        <v>0.1559748444180542</v>
       </c>
       <c r="E30" t="n">
-        <v>1041.9984</v>
+        <v>0.02432815209123622</v>
       </c>
     </row>
     <row r="31">
@@ -961,13 +961,13 @@
         <v>32.45</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>32.75777595936748</v>
       </c>
       <c r="D31" t="n">
-        <v>-32.45</v>
+        <v>0.3077759593674756</v>
       </c>
       <c r="E31" t="n">
-        <v>1053.0025</v>
+        <v>0.09472604116456999</v>
       </c>
     </row>
     <row r="32">
@@ -978,13 +978,13 @@
         <v>32.85</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>34.12422113804068</v>
       </c>
       <c r="D32" t="n">
-        <v>-32.85</v>
+        <v>1.27422113804068</v>
       </c>
       <c r="E32" t="n">
-        <v>1079.1225</v>
+        <v>1.623639508629686</v>
       </c>
     </row>
     <row r="33">
@@ -995,13 +995,13 @@
         <v>32.9</v>
       </c>
       <c r="C33" t="n">
-        <v>0</v>
+        <v>33.96927027946951</v>
       </c>
       <c r="D33" t="n">
-        <v>-32.9</v>
+        <v>1.069270279469514</v>
       </c>
       <c r="E33" t="n">
-        <v>1082.41</v>
+        <v>1.143338930556812</v>
       </c>
     </row>
     <row r="34">
@@ -1012,13 +1012,13 @@
         <v>33.1</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>33.53024531804003</v>
       </c>
       <c r="D34" t="n">
-        <v>-33.1</v>
+        <v>0.4302453180400292</v>
       </c>
       <c r="E34" t="n">
-        <v>1095.61</v>
+        <v>0.1851110336953659</v>
       </c>
     </row>
     <row r="35">
@@ -1029,13 +1029,13 @@
         <v>33.4</v>
       </c>
       <c r="C35" t="n">
-        <v>0</v>
+        <v>32.84650728479531</v>
       </c>
       <c r="D35" t="n">
-        <v>-33.4</v>
+        <v>-0.5534927152046905</v>
       </c>
       <c r="E35" t="n">
-        <v>1115.56</v>
+        <v>0.3063541857846606</v>
       </c>
     </row>
     <row r="36">
@@ -1046,13 +1046,13 @@
         <v>33.7</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>34.00686701367583</v>
       </c>
       <c r="D36" t="n">
-        <v>-33.7</v>
+        <v>0.3068670136758271</v>
       </c>
       <c r="E36" t="n">
-        <v>1135.69</v>
+        <v>0.09416736408232028</v>
       </c>
     </row>
     <row r="37">
@@ -1063,13 +1063,13 @@
         <v>34.1</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>34.89016021427642</v>
       </c>
       <c r="D37" t="n">
-        <v>-34.1</v>
+        <v>0.790160214276419</v>
       </c>
       <c r="E37" t="n">
-        <v>1162.81</v>
+        <v>0.6243531642253565</v>
       </c>
     </row>
     <row r="38">
@@ -1080,13 +1080,13 @@
         <v>34.4</v>
       </c>
       <c r="C38" t="n">
-        <v>0</v>
+        <v>35.13709982289468</v>
       </c>
       <c r="D38" t="n">
-        <v>-34.4</v>
+        <v>0.7370998228946846</v>
       </c>
       <c r="E38" t="n">
-        <v>1183.36</v>
+        <v>0.5433161489113754</v>
       </c>
     </row>
     <row r="39">
@@ -1097,13 +1097,13 @@
         <v>34.9</v>
       </c>
       <c r="C39" t="n">
-        <v>0</v>
+        <v>35.28494508555107</v>
       </c>
       <c r="D39" t="n">
-        <v>-34.9</v>
+        <v>0.3849450855510739</v>
       </c>
       <c r="E39" t="n">
-        <v>1218.01</v>
+        <v>0.1481827188899236</v>
       </c>
     </row>
     <row r="40">
@@ -1114,13 +1114,13 @@
         <v>35.3</v>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>34.84355280154394</v>
       </c>
       <c r="D40" t="n">
-        <v>-35.3</v>
+        <v>-0.4564471984560612</v>
       </c>
       <c r="E40" t="n">
-        <v>1246.09</v>
+        <v>0.2083440449783869</v>
       </c>
     </row>
     <row r="41">
@@ -1131,13 +1131,13 @@
         <v>35.7</v>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>35.66862906993612</v>
       </c>
       <c r="D41" t="n">
-        <v>-35.7</v>
+        <v>-0.03137093006388625</v>
       </c>
       <c r="E41" t="n">
-        <v>1274.49</v>
+        <v>0.0009841352530732422</v>
       </c>
     </row>
     <row r="42">
@@ -1148,13 +1148,13 @@
         <v>36.3</v>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>35.85962750787648</v>
       </c>
       <c r="D42" t="n">
-        <v>-36.3</v>
+        <v>-0.4403724921235153</v>
       </c>
       <c r="E42" t="n">
-        <v>1317.69</v>
+        <v>0.1939279318190755</v>
       </c>
     </row>
     <row r="43">
@@ -1165,13 +1165,13 @@
         <v>36.8</v>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>36.58988521355371</v>
       </c>
       <c r="D43" t="n">
-        <v>-36.8</v>
+        <v>-0.2101147864462831</v>
       </c>
       <c r="E43" t="n">
-        <v>1354.24</v>
+        <v>0.04414822348336716</v>
       </c>
     </row>
     <row r="44">
@@ -1182,13 +1182,13 @@
         <v>37.3</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>37.83083254539498</v>
       </c>
       <c r="D44" t="n">
-        <v>-37.3</v>
+        <v>0.5308325453949863</v>
       </c>
       <c r="E44" t="n">
-        <v>1391.29</v>
+        <v>0.2817831912505201</v>
       </c>
     </row>
     <row r="45">
@@ -1199,13 +1199,13 @@
         <v>37.9</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>39.01314395352769</v>
       </c>
       <c r="D45" t="n">
-        <v>-37.9</v>
+        <v>1.11314395352769</v>
       </c>
       <c r="E45" t="n">
-        <v>1436.41</v>
+        <v>1.239089461275255</v>
       </c>
     </row>
     <row r="46">
@@ -1216,13 +1216,13 @@
         <v>38.5</v>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>39.25621049148977</v>
       </c>
       <c r="D46" t="n">
-        <v>-38.5</v>
+        <v>0.7562104914897674</v>
       </c>
       <c r="E46" t="n">
-        <v>1482.25</v>
+        <v>0.5718543074391955</v>
       </c>
     </row>
     <row r="47">
@@ -1233,13 +1233,13 @@
         <v>38.9</v>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>39.2911214137161</v>
       </c>
       <c r="D47" t="n">
-        <v>-38.9</v>
+        <v>0.3911214137160997</v>
       </c>
       <c r="E47" t="n">
-        <v>1513.21</v>
+        <v>0.1529759602672804</v>
       </c>
     </row>
     <row r="48">
@@ -1250,13 +1250,13 @@
         <v>39.4</v>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>40.10510052842852</v>
       </c>
       <c r="D48" t="n">
-        <v>-39.4</v>
+        <v>0.7051005284285239</v>
       </c>
       <c r="E48" t="n">
-        <v>1552.36</v>
+        <v>0.4971667551901836</v>
       </c>
     </row>
     <row r="49">
@@ -1267,13 +1267,13 @@
         <v>39.9</v>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>39.87448722716134</v>
       </c>
       <c r="D49" t="n">
-        <v>-39.9</v>
+        <v>-0.02551277283865971</v>
       </c>
       <c r="E49" t="n">
-        <v>1592.01</v>
+        <v>0.0006509015779170528</v>
       </c>
     </row>
     <row r="50">
@@ -1284,13 +1284,13 @@
         <v>40.1</v>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>36.32202583591969</v>
       </c>
       <c r="D50" t="n">
-        <v>-40.1</v>
+        <v>-3.777974164080312</v>
       </c>
       <c r="E50" t="n">
-        <v>1608.01</v>
+        <v>14.27308878445833</v>
       </c>
     </row>
     <row r="51">
@@ -1301,13 +1301,13 @@
         <v>40.6</v>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>39.63872335809702</v>
       </c>
       <c r="D51" t="n">
-        <v>-40.6</v>
+        <v>-0.9612766419029768</v>
       </c>
       <c r="E51" t="n">
-        <v>1648.36</v>
+        <v>0.9240527822682639</v>
       </c>
     </row>
     <row r="52">
@@ -1318,11 +1318,11 @@
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="n">
-        <v>-1641.03</v>
+        <v>8.072418978433124</v>
       </c>
       <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>54420.1889</v>
+        <v>30.08121531779148</v>
       </c>
     </row>
     <row r="53">
@@ -1335,7 +1335,7 @@
       <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>1088.403778</v>
+        <v>0.6016243063558295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>